<commit_message>
remove all button added
</commit_message>
<xml_diff>
--- a/saved_schedules/esports_lounge_current.xlsx
+++ b/saved_schedules/esports_lounge_current.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,73 +470,56 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dummy Test</t>
+          <t>Nikko Sandgren</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Weekend Test</t>
+          <t>Jullian Kemp</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>9:00 PM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Olivia Schindler</t>
+          <t>Zion Williams</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>9:00 PM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>11:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
-        <is>
-          <t>Nikko Sandgren</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>11:00 PM</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>12:00 PM</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
         <is>
           <t>Olivia Schindler</t>
         </is>
@@ -553,7 +536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,80 +569,29 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Alan Haim</t>
+          <t>Greg Aiv</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tatiana Mata Diaz</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>6:00 PM</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>8:00 PM</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>Krish Chawla</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>8:00 PM</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>10:00 PM</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Zion Williams</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>10:00 PM</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>12:00 PM</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Test Worker</t>
         </is>
       </c>
     </row>
@@ -712,7 +644,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Jullian Kemp</t>
+          <t>Sebastian Hurd</t>
         </is>
       </c>
     </row>
@@ -724,19 +656,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>9:00 PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Daniel Finn</t>
+          <t>Jullian Kemp</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>9:00 PM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -746,7 +678,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Gissel O Rosa</t>
+          <t>Daniel Finn</t>
         </is>
       </c>
     </row>
@@ -794,53 +726,53 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Brooke Kazmierczak</t>
+          <t>Alan Haim</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9:00 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Greg Aiv</t>
+          <t>Zion Williams</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>9:00 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>11:00 PM</t>
+          <t>10:00 PM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Zion Williams</t>
+          <t>Gissel O Rosa</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>11:00 PM</t>
+          <t>10:00 PM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -850,7 +782,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Alan Haim</t>
+          <t>Brooke Kazmierczak</t>
         </is>
       </c>
     </row>
@@ -865,7 +797,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -898,46 +830,63 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Regenae Walkters</t>
+          <t>Daniel Senn</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Daniel Senn</t>
+          <t>Regenae Walkters</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>8:00 PM</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>10:00 PM</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>12:00 PM</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Gissel O Rosa</t>
+          <t>Daniel Senn</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>10:00 PM</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>12:00 PM</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Olivia Schindler</t>
         </is>
       </c>
     </row>
@@ -985,7 +934,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -997,24 +946,24 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jullian Kemp</t>
+          <t>Gissel O Rosa</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1072,53 +1021,53 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Test Worker</t>
+          <t>Tatiana Mata Diaz</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tatiana Mata Diaz</t>
+          <t>Daniel Finn</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sebastian Hurd</t>
+          <t>Brooke Kazmierczak</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1128,7 +1077,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Brooke Kazmierczak</t>
+          <t>Sebastian Hurd</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1092,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1176,210 +1125,210 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Dummy Test</t>
+          <t>Jash Hitesh Parekh</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Weekend Test</t>
+          <t>Gissel O Rosa</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Olivia Schindler</t>
+          <t>Krish Chawla</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>11:00 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Nikko Sandgren</t>
+          <t>Tatiana Mata Diaz</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>11:00 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Olivia Schindler</t>
+          <t>Daniel Finn</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Jullian Kemp</t>
+          <t>Brooke Kazmierczak</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>11:00 PM</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Daniel Finn</t>
+          <t>Sebastian Hurd</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Gissel O Rosa</t>
+          <t>Nikko Sandgren</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Brooke Kazmierczak</t>
+          <t>Jullian Kemp</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1389,14 +1338,14 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Greg Aiv</t>
+          <t>Zion Williams</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1406,12 +1355,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Zion Williams</t>
+          <t>Olivia Schindler</t>
         </is>
       </c>
     </row>
@@ -1423,12 +1372,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1440,330 +1389,264 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Test Worker</t>
+          <t>Zion Williams</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>10:00 PM</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Tatiana Mata Diaz</t>
+          <t>Gissel O Rosa</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>10:00 PM</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Sebastian Hurd</t>
+          <t>Brooke Kazmierczak</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Brooke Kazmierczak</t>
+          <t>Sebastian Hurd</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>9:00 PM</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Regenae Walkters</t>
+          <t>Jullian Kemp</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>9:00 PM</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Daniel Senn</t>
+          <t>Daniel Finn</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Gissel O Rosa</t>
+          <t>Greg Aiv</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Jash Hitesh Parekh</t>
+          <t>Krish Chawla</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Jullian Kemp</t>
+          <t>Daniel Senn</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>10:00 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Krish Chawla</t>
+          <t>Regenae Walkters</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>4:00 PM</t>
+          <t>10:00 PM</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Alan Haim</t>
+          <t>Daniel Senn</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4:00 PM</t>
+          <t>10:00 PM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Tatiana Mata Diaz</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>6:00 PM</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>8:00 PM</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Krish Chawla</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>8:00 PM</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>10:00 PM</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Zion Williams</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>10:00 PM</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>12:00 PM</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Test Worker</t>
+          <t>Olivia Schindler</t>
         </is>
       </c>
     </row>

</xml_diff>